<commit_message>
Almost Final framework is commiting.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -14,48 +14,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>TestCaseId</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>EmailId</t>
-  </si>
-  <si>
-    <t>ashish12psitsrivastava@gmail.com</t>
-  </si>
-  <si>
-    <t>SignIn_01</t>
-  </si>
-  <si>
-    <t>SignIn_02</t>
-  </si>
-  <si>
-    <t>SignIn_03</t>
-  </si>
-  <si>
-    <t>SignIn_04</t>
-  </si>
-  <si>
-    <t>SignIn_05</t>
-  </si>
-  <si>
-    <t>Ashish_01</t>
-  </si>
-  <si>
-    <t>Ashish_02</t>
-  </si>
-  <si>
-    <t>Ashish_03</t>
-  </si>
-  <si>
-    <t>Ashish_04</t>
-  </si>
-  <si>
-    <t>Ashish_05</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+  <si>
+    <t>ashitestmail@gmail.com</t>
+  </si>
+  <si>
+    <t>researcher</t>
+  </si>
+  <si>
+    <t>Gmail/LoginEmailId</t>
+  </si>
+  <si>
+    <t>Gmail/LoginPassword</t>
+  </si>
+  <si>
+    <t>TestCase_01</t>
+  </si>
+  <si>
+    <t>TestCase_02</t>
+  </si>
+  <si>
+    <t>TestCase_03</t>
+  </si>
+  <si>
+    <t>TestCase_04</t>
+  </si>
+  <si>
+    <t>TestCase_05</t>
+  </si>
+  <si>
+    <t>TestCase_Id</t>
   </si>
 </sst>
 </file>
@@ -408,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -417,79 +405,84 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="ashish@12psitsrivastava@gmail.com"/>
     <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="B3:B6" r:id="rId3" display="ashish12psitsrivastava@gmail.com"/>
+    <hyperlink ref="B3:B6" r:id="rId3" display="ashitestmail@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>